<commit_message>
sửa lại update file và xem danh sách sinh viên của các phòng
</commit_message>
<xml_diff>
--- a/Design document/Excels/khen_thuong_doan.xlsx
+++ b/Design document/Excels/khen_thuong_doan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="63">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">K59CA</t>
   </si>
   <si>
-    <t xml:space="preserve">gioi</t>
+    <t xml:space="preserve">Giỏi</t>
   </si>
   <si>
     <t xml:space="preserve">Nguyễn Phạm Thiện Dũng</t>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Trần Trọng Đạt</t>
   </si>
   <si>
+    <t xml:space="preserve">Khá</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nguyễn Trọng Đông</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nguyễn Hoàng Hải</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xuất Sắc</t>
   </si>
   <si>
     <t xml:space="preserve">Chu Viết Hiếu</t>
@@ -383,18 +389,18 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28:F52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,7 +423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -437,7 +443,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -457,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -474,10 +480,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -485,7 +491,7 @@
         <v>14020791</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>35290</v>
@@ -494,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -505,7 +511,7 @@
         <v>14020783</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>35345</v>
@@ -517,7 +523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -525,7 +531,7 @@
         <v>14020792</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="n">
         <v>35425</v>
@@ -534,10 +540,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -545,7 +551,7 @@
         <v>14020163</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>35355</v>
@@ -557,7 +563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
@@ -565,7 +571,7 @@
         <v>14020190</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>35126</v>
@@ -577,7 +583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -585,7 +591,7 @@
         <v>14020663</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5" t="n">
         <v>35360</v>
@@ -594,10 +600,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
@@ -605,7 +611,7 @@
         <v>14020198</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>35347</v>
@@ -614,10 +620,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
@@ -625,7 +631,7 @@
         <v>14020208</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5" t="n">
         <v>35209</v>
@@ -637,7 +643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -645,7 +651,7 @@
         <v>14020664</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>35207</v>
@@ -654,10 +660,10 @@
         <v>7</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -665,19 +671,19 @@
         <v>14020652</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D14" s="7" t="n">
         <v>35176</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
@@ -685,19 +691,19 @@
         <v>14020025</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="7" t="n">
         <v>35288</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
@@ -705,19 +711,19 @@
         <v>14020653</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D16" s="7" t="n">
         <v>35255</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
@@ -725,19 +731,19 @@
         <v>14020576</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="7" t="n">
         <v>35266</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
@@ -745,19 +751,19 @@
         <v>14020038</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D18" s="7" t="n">
         <v>35382</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
@@ -765,19 +771,19 @@
         <v>14020039</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D19" s="7" t="n">
         <v>35088</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
@@ -785,19 +791,19 @@
         <v>14020578</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D20" s="7" t="n">
         <v>35075</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
@@ -805,19 +811,19 @@
         <v>14020061</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D21" s="7" t="n">
         <v>35112</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
@@ -825,19 +831,19 @@
         <v>14020818</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D22" s="7" t="n">
         <v>35024</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
@@ -845,19 +851,19 @@
         <v>14020064</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D23" s="7" t="n">
         <v>35253</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
@@ -865,19 +871,19 @@
         <v>14020088</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D24" s="7" t="n">
         <v>35375</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
@@ -885,19 +891,19 @@
         <v>14020582</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D25" s="7" t="n">
         <v>35289</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
@@ -905,19 +911,19 @@
         <v>14020116</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D26" s="7" t="n">
         <v>35226</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
@@ -925,13 +931,13 @@
         <v>14020658</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D27" s="7" t="n">
         <v>35429</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>8</v>
@@ -945,16 +951,16 @@
         <v>14020585</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D28" s="7" t="n">
         <v>35236</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,16 +971,16 @@
         <v>14020146</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D29" s="7" t="n">
         <v>35362</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,13 +991,13 @@
         <v>14020661</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D30" s="7" t="n">
         <v>35151</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>8</v>
@@ -1005,16 +1011,16 @@
         <v>14020155</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D31" s="7" t="n">
         <v>35212</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,13 +1031,13 @@
         <v>14020161</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D32" s="7" t="n">
         <v>34823</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>8</v>
@@ -1045,13 +1051,13 @@
         <v>14020056</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D33" s="10" t="n">
         <v>35069</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>8</v>
@@ -1065,16 +1071,16 @@
         <v>14020066</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>35376</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,16 +1091,16 @@
         <v>14020084</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>35300</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,13 +1111,13 @@
         <v>14020091</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D36" s="10" t="n">
         <v>35355</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>8</v>
@@ -1125,16 +1131,16 @@
         <v>14020102</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>35343</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,13 +1151,13 @@
         <v>14020123</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D38" s="10" t="n">
         <v>35253</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>8</v>
@@ -1165,13 +1171,13 @@
         <v>14020131</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>35154</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>8</v>
@@ -1185,16 +1191,16 @@
         <v>14020139</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D40" s="10" t="n">
         <v>35414</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,16 +1211,16 @@
         <v>14020180</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D41" s="10" t="n">
         <v>35072</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,13 +1231,13 @@
         <v>14020169</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D42" s="10" t="n">
         <v>35417</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>8</v>
@@ -1245,16 +1251,16 @@
         <v>14020170</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D43" s="10" t="n">
         <v>35242</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,13 +1271,13 @@
         <v>14020213</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D44" s="10" t="n">
         <v>35197</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>8</v>
@@ -1285,13 +1291,13 @@
         <v>14020225</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D45" s="10" t="n">
         <v>35072</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>8</v>
@@ -1305,16 +1311,16 @@
         <v>14020234</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D46" s="10" t="n">
         <v>35120</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1325,16 +1331,16 @@
         <v>14020249</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D47" s="10" t="n">
         <v>35414</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,13 +1351,13 @@
         <v>14020752</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D48" s="10" t="n">
         <v>35373</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>8</v>
@@ -1365,16 +1371,16 @@
         <v>14020629</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D49" s="10" t="n">
         <v>35141</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,13 +1391,13 @@
         <v>14020669</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D50" s="10" t="n">
         <v>35383</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>8</v>
@@ -1405,13 +1411,13 @@
         <v>14020266</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D51" s="10" t="n">
         <v>35145</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>8</v>
@@ -1425,16 +1431,16 @@
         <v>14020268</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D52" s="10" t="n">
         <v>35419</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>